<commit_message>
FHT64 model in matlab is working
</commit_message>
<xml_diff>
--- a/fht/5stage_fht64.xlsx
+++ b/fht/5stage_fht64.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\fft\fht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SS\fpga\fft\fht\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>x1</t>
   </si>
@@ -37,12 +37,66 @@
   <si>
     <t>cos</t>
   </si>
+  <si>
+    <t xml:space="preserve"> +step</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -step</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +3*step</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -3*step</t>
+  </si>
+  <si>
+    <t>bank(1-4)</t>
+  </si>
+  <si>
+    <t>row(1-16)</t>
+  </si>
+  <si>
+    <t>j(1-16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +7*step</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +5*step</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -5*step</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -7*step</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +15*step</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +13*step</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -13*step</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -15*step</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>cos mirror</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,6 +104,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -68,12 +129,211 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -354,25 +614,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="Q10" sqref="Q10:S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -387,19 +647,40 @@
       <c r="H1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <f>A2+1</f>
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="10">
         <v>0</v>
       </c>
       <c r="E2">
@@ -415,19 +696,58 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B5" si="0">A3+1</f>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="L2" s="6">
+        <v>1</v>
+      </c>
+      <c r="M2" t="str">
+        <f>DEC2BIN(D2,5)</f>
+        <v>00000</v>
+      </c>
+      <c r="N2" s="24">
+        <f>SUMPRODUCT(MID($M2,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>BIN2DEC(N2)</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>DEC2BIN(P2,4)</f>
+        <v>0000</v>
+      </c>
+      <c r="R2">
+        <f>SUMPRODUCT(MID($Q2,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <f>BIN2DEC(R2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <f t="shared" ref="B3:B4" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="10">
         <v>16</v>
       </c>
       <c r="E3">
@@ -443,19 +763,55 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="J3" s="4">
+        <v>2</v>
+      </c>
+      <c r="K3" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="L3" s="6">
+        <v>1</v>
+      </c>
+      <c r="M3" t="str">
+        <f>DEC2BIN(D3,5)</f>
+        <v>10000</v>
+      </c>
+      <c r="N3" s="24">
+        <f>SUMPRODUCT(MID($M3,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O33" si="2">BIN2DEC(N3)</f>
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>8</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q8" si="3">DEC2BIN(P3,4)</f>
+        <v>1000</v>
+      </c>
+      <c r="R3">
+        <f>SUMPRODUCT(MID($Q3,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S8" si="4">BIN2DEC(R3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="10">
         <v>8</v>
       </c>
       <c r="E4">
@@ -471,19 +827,58 @@
       <c r="H4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4" s="14">
+        <v>3</v>
+      </c>
+      <c r="K4" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="str">
+        <f>DEC2BIN(D4,5)</f>
+        <v>01000</v>
+      </c>
+      <c r="N4" s="24">
+        <f>SUMPRODUCT(MID($M4,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>10</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>4</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="3"/>
+        <v>0100</v>
+      </c>
+      <c r="R4">
+        <f>SUMPRODUCT(MID($Q4,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>10</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>6</v>
       </c>
-      <c r="B5">
-        <f>A5+1</f>
+      <c r="B5" s="5">
+        <f t="shared" ref="B5:B33" si="5">A5+1</f>
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="10">
         <v>24</v>
       </c>
       <c r="E5">
@@ -499,19 +894,55 @@
       <c r="H5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="J5" s="4">
+        <v>4</v>
+      </c>
+      <c r="K5" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" t="str">
+        <f>DEC2BIN(D5,5)</f>
+        <v>11000</v>
+      </c>
+      <c r="N5" s="24">
+        <f>SUMPRODUCT(MID($M5,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>11</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>12</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="3"/>
+        <v>1100</v>
+      </c>
+      <c r="R5">
+        <f>SUMPRODUCT(MID($Q5,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>11</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>8</v>
       </c>
-      <c r="B6">
-        <f>A6+1</f>
+      <c r="B6" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>15</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="10">
         <v>4</v>
       </c>
       <c r="E6">
@@ -527,19 +958,58 @@
       <c r="H6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="14">
+        <v>5</v>
+      </c>
+      <c r="K6" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" t="str">
+        <f>DEC2BIN(D6,5)</f>
+        <v>00100</v>
+      </c>
+      <c r="N6" s="24">
+        <f>SUMPRODUCT(MID($M6,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>100</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="3"/>
+        <v>0010</v>
+      </c>
+      <c r="R6">
+        <f>SUMPRODUCT(MID($Q6,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>100</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>10</v>
       </c>
-      <c r="B7">
-        <f>A7+1</f>
+      <c r="B7" s="5">
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>13</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="10">
         <v>20</v>
       </c>
       <c r="E7">
@@ -555,19 +1025,55 @@
       <c r="H7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="J7" s="4">
+        <v>6</v>
+      </c>
+      <c r="K7" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" t="str">
+        <f>DEC2BIN(D7,5)</f>
+        <v>10100</v>
+      </c>
+      <c r="N7" s="24">
+        <f>SUMPRODUCT(MID($M7,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>101</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>10</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="3"/>
+        <v>1010</v>
+      </c>
+      <c r="R7">
+        <f>SUMPRODUCT(MID($Q7,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>101</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>12</v>
       </c>
-      <c r="B8">
-        <f>A8+1</f>
+      <c r="B8" s="5">
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>11</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="10">
         <v>12</v>
       </c>
       <c r="E8">
@@ -583,19 +1089,55 @@
       <c r="H8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="J8" s="4">
+        <v>7</v>
+      </c>
+      <c r="K8" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" t="str">
+        <f>DEC2BIN(D8,5)</f>
+        <v>01100</v>
+      </c>
+      <c r="N8" s="24">
+        <f>SUMPRODUCT(MID($M8,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>110</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>6</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="3"/>
+        <v>0110</v>
+      </c>
+      <c r="R8">
+        <f>SUMPRODUCT(MID($Q8,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>110</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>14</v>
       </c>
-      <c r="B9">
-        <f>A9+1</f>
+      <c r="B9" s="5">
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>9</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="10">
         <v>28</v>
       </c>
       <c r="E9">
@@ -611,19 +1153,40 @@
       <c r="H9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="J9" s="4">
+        <v>8</v>
+      </c>
+      <c r="K9" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" t="str">
+        <f>DEC2BIN(D9,5)</f>
+        <v>11100</v>
+      </c>
+      <c r="N9" s="24">
+        <f>SUMPRODUCT(MID($M9,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>111</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>16</v>
       </c>
-      <c r="B10">
-        <f>A10+1</f>
+      <c r="B10" s="5">
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>31</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="10">
         <v>2</v>
       </c>
       <c r="E10">
@@ -639,19 +1202,43 @@
       <c r="H10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10" s="14">
+        <v>9</v>
+      </c>
+      <c r="K10" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" t="str">
+        <f>DEC2BIN(D10,5)</f>
+        <v>00010</v>
+      </c>
+      <c r="N10" s="24">
+        <f>SUMPRODUCT(MID($M10,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>1000</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>18</v>
       </c>
-      <c r="B11">
-        <f>A11+1</f>
+      <c r="B11" s="5">
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>29</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="10">
         <v>18</v>
       </c>
       <c r="E11">
@@ -667,19 +1254,40 @@
       <c r="H11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="J11" s="4">
+        <v>10</v>
+      </c>
+      <c r="K11" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" t="str">
+        <f>DEC2BIN(D11,5)</f>
+        <v>10010</v>
+      </c>
+      <c r="N11" s="24">
+        <f>SUMPRODUCT(MID($M11,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>1001</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>20</v>
       </c>
-      <c r="B12">
-        <f>A12+1</f>
+      <c r="B12" s="5">
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>27</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="10">
         <v>10</v>
       </c>
       <c r="E12">
@@ -695,19 +1303,40 @@
       <c r="H12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="J12" s="4">
+        <v>11</v>
+      </c>
+      <c r="K12" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" t="str">
+        <f>DEC2BIN(D12,5)</f>
+        <v>01010</v>
+      </c>
+      <c r="N12" s="24">
+        <f>SUMPRODUCT(MID($M12,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>1010</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>22</v>
       </c>
-      <c r="B13">
-        <f>A13+1</f>
+      <c r="B13" s="5">
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>25</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="10">
         <v>26</v>
       </c>
       <c r="E13">
@@ -723,19 +1352,40 @@
       <c r="H13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="J13" s="4">
+        <v>12</v>
+      </c>
+      <c r="K13" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" t="str">
+        <f>DEC2BIN(D13,5)</f>
+        <v>11010</v>
+      </c>
+      <c r="N13" s="24">
+        <f>SUMPRODUCT(MID($M13,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>1011</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>24</v>
       </c>
-      <c r="B14">
-        <f>A14+1</f>
+      <c r="B14" s="5">
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>23</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="10">
         <v>6</v>
       </c>
       <c r="E14">
@@ -751,19 +1401,40 @@
       <c r="H14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="J14" s="4">
+        <v>13</v>
+      </c>
+      <c r="K14" s="12">
+        <v>3.1</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" t="str">
+        <f>DEC2BIN(D14,5)</f>
+        <v>00110</v>
+      </c>
+      <c r="N14" s="24">
+        <f>SUMPRODUCT(MID($M14,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>1100</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>26</v>
       </c>
-      <c r="B15">
-        <f>A15+1</f>
+      <c r="B15" s="5">
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>21</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="10">
         <v>22</v>
       </c>
       <c r="E15">
@@ -779,19 +1450,40 @@
       <c r="H15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="J15" s="4">
+        <v>14</v>
+      </c>
+      <c r="K15" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" t="str">
+        <f>DEC2BIN(D15,5)</f>
+        <v>10110</v>
+      </c>
+      <c r="N15" s="24">
+        <f>SUMPRODUCT(MID($M15,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>1101</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>28</v>
       </c>
-      <c r="B16">
-        <f>A16+1</f>
+      <c r="B16" s="5">
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>19</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="10">
         <v>14</v>
       </c>
       <c r="E16">
@@ -807,19 +1499,40 @@
       <c r="H16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="J16" s="4">
+        <v>15</v>
+      </c>
+      <c r="K16" s="12">
+        <v>3.1</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" t="str">
+        <f>DEC2BIN(D16,5)</f>
+        <v>01110</v>
+      </c>
+      <c r="N16" s="24">
+        <f>SUMPRODUCT(MID($M16,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>1110</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>30</v>
       </c>
-      <c r="B17">
-        <f>A17+1</f>
+      <c r="B17" s="5">
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="5">
         <v>17</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="10">
         <v>30</v>
       </c>
       <c r="E17">
@@ -835,19 +1548,40 @@
       <c r="H17">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="J17" s="4">
+        <v>16</v>
+      </c>
+      <c r="K17" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" t="str">
+        <f>DEC2BIN(D17,5)</f>
+        <v>11110</v>
+      </c>
+      <c r="N17" s="24">
+        <f>SUMPRODUCT(MID($M17,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>1111</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>32</v>
       </c>
-      <c r="B18">
-        <f>A18+1</f>
+      <c r="B18" s="5">
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <v>63</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="10">
         <v>1</v>
       </c>
       <c r="E18">
@@ -863,19 +1597,41 @@
       <c r="H18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="I18">
+        <v>16</v>
+      </c>
+      <c r="J18" s="21">
+        <v>17</v>
+      </c>
+      <c r="K18" s="15"/>
+      <c r="L18" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M18" t="str">
+        <f>DEC2BIN(D18,5)</f>
+        <v>00001</v>
+      </c>
+      <c r="N18" s="24">
+        <f>SUMPRODUCT(MID($M18,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>10000</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>34</v>
       </c>
-      <c r="B19">
-        <f>A19+1</f>
+      <c r="B19" s="5">
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <v>61</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="10">
         <v>17</v>
       </c>
       <c r="E19">
@@ -891,19 +1647,38 @@
       <c r="H19">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="J19" s="19">
+        <v>18</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="M19" t="str">
+        <f>DEC2BIN(D19,5)</f>
+        <v>10001</v>
+      </c>
+      <c r="N19" s="24">
+        <f>SUMPRODUCT(MID($M19,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>10001</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>36</v>
       </c>
-      <c r="B20">
-        <f>A20+1</f>
+      <c r="B20" s="5">
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="5">
         <v>59</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="10">
         <v>9</v>
       </c>
       <c r="E20">
@@ -919,17 +1694,39 @@
       <c r="H20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="J20" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20" t="str">
+        <f>DEC2BIN(D20,5)</f>
+        <v>01001</v>
+      </c>
+      <c r="N20" s="24">
+        <f>SUMPRODUCT(MID($M20,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>10010</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>38</v>
       </c>
-      <c r="B21">
-        <f>A21+1</f>
+      <c r="B21" s="5">
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="5">
         <v>57</v>
+      </c>
+      <c r="D21" s="10">
+        <v>25</v>
       </c>
       <c r="E21">
         <v>50</v>
@@ -944,17 +1741,39 @@
       <c r="H21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="J21" s="23">
+        <v>23</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M21" t="str">
+        <f>DEC2BIN(D21,5)</f>
+        <v>11001</v>
+      </c>
+      <c r="N21" s="24">
+        <f>SUMPRODUCT(MID($M21,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>10011</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>40</v>
       </c>
-      <c r="B22">
-        <f>A22+1</f>
+      <c r="B22" s="5">
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="5">
         <v>55</v>
+      </c>
+      <c r="D22" s="10">
+        <v>5</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -969,17 +1788,39 @@
       <c r="H22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="J22" s="23">
+        <v>24</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" t="str">
+        <f>DEC2BIN(D22,5)</f>
+        <v>00101</v>
+      </c>
+      <c r="N22" s="24">
+        <f>SUMPRODUCT(MID($M22,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>10100</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>42</v>
       </c>
-      <c r="B23">
-        <f>A23+1</f>
+      <c r="B23" s="5">
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="5">
         <v>53</v>
+      </c>
+      <c r="D23" s="10">
+        <v>21</v>
       </c>
       <c r="E23">
         <v>42</v>
@@ -994,17 +1835,39 @@
       <c r="H23">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="J23" s="23">
+        <v>25</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M23" t="str">
+        <f>DEC2BIN(D23,5)</f>
+        <v>10101</v>
+      </c>
+      <c r="N23" s="24">
+        <f>SUMPRODUCT(MID($M23,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>10101</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>44</v>
       </c>
-      <c r="B24">
-        <f>A24+1</f>
+      <c r="B24" s="5">
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="5">
         <v>51</v>
+      </c>
+      <c r="D24" s="10">
+        <v>13</v>
       </c>
       <c r="E24">
         <v>26</v>
@@ -1019,17 +1882,39 @@
       <c r="H24">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="J24" s="23">
+        <v>26</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" t="str">
+        <f>DEC2BIN(D24,5)</f>
+        <v>01101</v>
+      </c>
+      <c r="N24" s="24">
+        <f>SUMPRODUCT(MID($M24,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>10110</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>46</v>
       </c>
-      <c r="B25">
-        <f>A25+1</f>
+      <c r="B25" s="5">
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="5">
         <v>49</v>
+      </c>
+      <c r="D25" s="10">
+        <v>29</v>
       </c>
       <c r="E25">
         <v>58</v>
@@ -1044,17 +1929,39 @@
       <c r="H25">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="J25" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="M25" t="str">
+        <f>DEC2BIN(D25,5)</f>
+        <v>11101</v>
+      </c>
+      <c r="N25" s="24">
+        <f>SUMPRODUCT(MID($M25,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>10111</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>48</v>
       </c>
-      <c r="B26">
-        <f>A26+1</f>
+      <c r="B26" s="5">
+        <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="5">
         <v>47</v>
+      </c>
+      <c r="D26" s="10">
+        <v>3</v>
       </c>
       <c r="E26">
         <v>6</v>
@@ -1069,17 +1976,39 @@
       <c r="H26">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="J26" s="4">
+        <v>31</v>
+      </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="M26" t="str">
+        <f>DEC2BIN(D26,5)</f>
+        <v>00011</v>
+      </c>
+      <c r="N26" s="24">
+        <f>SUMPRODUCT(MID($M26,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>11000</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
         <v>50</v>
       </c>
-      <c r="B27">
-        <f>A27+1</f>
+      <c r="B27" s="5">
+        <f t="shared" si="5"/>
         <v>51</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="5">
         <v>45</v>
+      </c>
+      <c r="D27" s="10">
+        <v>19</v>
       </c>
       <c r="E27">
         <v>38</v>
@@ -1094,17 +2023,39 @@
       <c r="H27">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="J27" s="7">
+        <v>32</v>
+      </c>
+      <c r="K27" s="8"/>
+      <c r="L27" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M27" t="str">
+        <f>DEC2BIN(D27,5)</f>
+        <v>10011</v>
+      </c>
+      <c r="N27" s="24">
+        <f>SUMPRODUCT(MID($M27,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>11001</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>52</v>
       </c>
-      <c r="B28">
-        <f>A28+1</f>
+      <c r="B28" s="5">
+        <f t="shared" si="5"/>
         <v>53</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="5">
         <v>43</v>
+      </c>
+      <c r="D28" s="10">
+        <v>11</v>
       </c>
       <c r="E28">
         <v>22</v>
@@ -1119,17 +2070,32 @@
       <c r="H28">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="M28" t="str">
+        <f>DEC2BIN(D28,5)</f>
+        <v>01011</v>
+      </c>
+      <c r="N28" s="24">
+        <f>SUMPRODUCT(MID($M28,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>11010</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>54</v>
       </c>
-      <c r="B29">
-        <f>A29+1</f>
+      <c r="B29" s="5">
+        <f t="shared" si="5"/>
         <v>55</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="5">
         <v>41</v>
+      </c>
+      <c r="D29" s="10">
+        <v>27</v>
       </c>
       <c r="E29">
         <v>54</v>
@@ -1144,17 +2110,32 @@
       <c r="H29">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="M29" t="str">
+        <f>DEC2BIN(D29,5)</f>
+        <v>11011</v>
+      </c>
+      <c r="N29" s="24">
+        <f>SUMPRODUCT(MID($M29,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>11011</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
         <v>56</v>
       </c>
-      <c r="B30">
-        <f>A30+1</f>
+      <c r="B30" s="5">
+        <f t="shared" si="5"/>
         <v>57</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="5">
         <v>39</v>
+      </c>
+      <c r="D30" s="10">
+        <v>7</v>
       </c>
       <c r="E30">
         <v>14</v>
@@ -1169,17 +2150,32 @@
       <c r="H30">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="M30" t="str">
+        <f>DEC2BIN(D30,5)</f>
+        <v>00111</v>
+      </c>
+      <c r="N30" s="24">
+        <f>SUMPRODUCT(MID($M30,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>11100</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>58</v>
       </c>
-      <c r="B31">
-        <f>A31+1</f>
+      <c r="B31" s="5">
+        <f t="shared" si="5"/>
         <v>59</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="5">
         <v>37</v>
+      </c>
+      <c r="D31" s="10">
+        <v>23</v>
       </c>
       <c r="E31">
         <v>46</v>
@@ -1194,17 +2190,32 @@
       <c r="H31">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="M31" t="str">
+        <f>DEC2BIN(D31,5)</f>
+        <v>10111</v>
+      </c>
+      <c r="N31" s="24">
+        <f>SUMPRODUCT(MID($M31,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>11101</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
         <v>60</v>
       </c>
-      <c r="B32">
-        <f>A32+1</f>
+      <c r="B32" s="5">
+        <f t="shared" si="5"/>
         <v>61</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="5">
         <v>35</v>
+      </c>
+      <c r="D32" s="10">
+        <v>15</v>
       </c>
       <c r="E32">
         <v>30</v>
@@ -1219,17 +2230,32 @@
       <c r="H32">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="M32" t="str">
+        <f>DEC2BIN(D32,5)</f>
+        <v>01111</v>
+      </c>
+      <c r="N32" s="24">
+        <f>SUMPRODUCT(MID($M32,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>11110</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
         <v>62</v>
       </c>
-      <c r="B33">
-        <f>A33+1</f>
+      <c r="B33" s="8">
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="8">
         <v>33</v>
+      </c>
+      <c r="D33" s="11">
+        <v>31</v>
       </c>
       <c r="E33">
         <v>62</v>
@@ -1244,8 +2270,21 @@
       <c r="H33">
         <v>31</v>
       </c>
+      <c r="M33" t="str">
+        <f>DEC2BIN(D33,5)</f>
+        <v>11111</v>
+      </c>
+      <c r="N33" s="24">
+        <f>SUMPRODUCT(MID($M33,{1;2;3;4;5},1)*10^{0;1;2;3;4})</f>
+        <v>11111</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>